<commit_message>
Test result grouping in real rendering
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DefaultReportGeneratorTest/TestRender.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DefaultReportGeneratorTest/TestRender.xlsx
@@ -123,8 +123,16 @@
     <x:numFmt numFmtId="0" formatCode=""/>
     <x:numFmt numFmtId="165" formatCode="#,0.00"/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="2">
     <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
@@ -159,24 +167,31 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
+  <x:cellXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -499,13 +514,14 @@
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
+      <x:c r="B3" s="0" t="s"/>
       <x:c r="C3" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="n">
+      <x:c r="E3" s="2" t="n">
         <x:v>55.76</x:v>
       </x:c>
       <x:c r="H3" s="0" t="n">
@@ -516,24 +532,26 @@
       </x:c>
     </x:row>
     <x:row r="4" spans="1:10">
+      <x:c r="B4" s="0" t="s"/>
       <x:c r="C4" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="n">
+      <x:c r="E4" s="2" t="n">
         <x:v>55.76</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:10">
+      <x:c r="B5" s="0" t="s"/>
       <x:c r="C5" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E5" s="0" t="n">
+      <x:c r="E5" s="2" t="n">
         <x:v>55.76</x:v>
       </x:c>
     </x:row>
@@ -554,28 +572,36 @@
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10">
+      <x:c r="B8" s="0" t="s"/>
       <x:c r="C8" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="E8" s="0" t="n">
+      <x:c r="E8" s="2" t="n">
         <x:v>5500.8</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:10">
+      <x:c r="B9" s="0" t="s"/>
       <x:c r="C9" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="E9" s="0" t="n">
+      <x:c r="E9" s="2" t="n">
         <x:v>5500.8</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
+  <x:mergeCells count="4">
+    <x:mergeCell ref="B3:B5"/>
+    <x:mergeCell ref="E3:E5"/>
+    <x:mergeCell ref="B8:B9"/>
+    <x:mergeCell ref="E8:E9"/>
+  </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
@@ -633,7 +659,7 @@
       <x:c r="D3" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="G3" s="2" t="n">
+      <x:c r="G3" s="3" t="n">
         <x:v>523635.93</x:v>
       </x:c>
       <x:c r="O3" s="0" t="n">
@@ -656,7 +682,7 @@
       <x:c r="F4" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="G4" s="2" t="s"/>
+      <x:c r="G4" s="3" t="s"/>
     </x:row>
     <x:row r="5" spans="1:25">
       <x:c r="B5" s="0" t="n">
@@ -668,12 +694,12 @@
       <x:c r="F5" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="G5" s="2" t="n">
+      <x:c r="G5" s="3" t="n">
         <x:v>100000.5532</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:25">
-      <x:c r="G6" s="2" t="n">
+      <x:c r="G6" s="3" t="n">
         <x:v>623636.4832</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Test change of self data item template
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/DefaultReportGeneratorTest/TestRender.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/DefaultReportGeneratorTest/TestRender.xlsx
@@ -615,7 +615,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:Y10"/>
+  <x:dimension ref="A1:Y21"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -733,6 +733,56 @@
         <x:v>31</x:v>
       </x:c>
     </x:row>
+    <x:row r="12" spans="1:25">
+      <x:c r="B12" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:25">
+      <x:c r="B13" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:25">
+      <x:c r="B14" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:25">
+      <x:c r="B15" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:25">
+      <x:c r="B16" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:25">
+      <x:c r="B17" s="0" t="n">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:25">
+      <x:c r="B18" s="0" t="n">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:25">
+      <x:c r="B19" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:25">
+      <x:c r="B20" s="0" t="n">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:25">
+      <x:c r="B21" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>